<commit_message>
update old list resource codes
</commit_message>
<xml_diff>
--- a/data/address/cn.v1.xlsx
+++ b/data/address/cn.v1.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11013"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12C1576C-A858-4D47-87C2-F7AF3603FED8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4245AE8-8AC0-5A41-86A5-88F49C8A5724}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3420" yWindow="2400" windowWidth="20940" windowHeight="14360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="china" sheetId="1" r:id="rId1"/>
-    <sheet name="taiwan" sheetId="2" r:id="rId2"/>
+    <sheet name="other" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -4758,8 +4758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CW373"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>

</xml_diff>